<commit_message>
work on intros and overall data
</commit_message>
<xml_diff>
--- a/source/Overall-figures.xlsx
+++ b/source/Overall-figures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="740" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -24,37 +24,37 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Asset Size</t>
+    <t>asset size</t>
   </si>
   <si>
-    <t>$ Amount Grants MN</t>
+    <t>dollars_mn</t>
   </si>
   <si>
-    <t>$ Amount Grants NYC</t>
+    <t>dollars_nyc</t>
   </si>
   <si>
-    <t>$ Amount Grants Other</t>
+    <t>dollars_other</t>
   </si>
   <si>
-    <t>Grants Total</t>
+    <t>dollars_total</t>
   </si>
   <si>
-    <t>$ Amount General Program</t>
+    <t>dollars_gp</t>
   </si>
   <si>
-    <t>$ Amount New York City Film and Video Program</t>
+    <t>dollars_nyc_fv</t>
   </si>
   <si>
-    <t>$ Amount Travel and Study Program</t>
+    <t>dollars_ts</t>
   </si>
   <si>
-    <t>$ Amount Minnesota Film and Video Program</t>
+    <t>dollars_mn_fv</t>
   </si>
   <si>
-    <t xml:space="preserve"># of Grant applications--all </t>
+    <t>applications</t>
   </si>
   <si>
-    <t># of Grants Approved--all</t>
+    <t>approved</t>
   </si>
 </sst>
 </file>
@@ -71,7 +71,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -484,8 +483,8 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L56" sqref="L56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -501,7 +500,7 @@
     <col min="13" max="13" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="100">
+    <row r="1" spans="1:13" ht="40">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +542,9 @@
       <c r="A2">
         <v>1964</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
       <c r="C2" s="6">
         <v>32684.84</v>
       </c>
@@ -579,7 +580,9 @@
       <c r="A3">
         <v>1965</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
       <c r="C3" s="6">
         <v>0</v>
       </c>
@@ -615,7 +618,9 @@
       <c r="A4">
         <v>1966</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
       <c r="C4" s="6">
         <v>14000</v>
       </c>
@@ -651,7 +656,9 @@
       <c r="A5">
         <v>1967</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
       <c r="C5" s="6">
         <v>18610</v>
       </c>

</xml_diff>